<commit_message>
added graph images to report
Co-Authored-By: Daniel <dnykja18@student.aau.dk>
</commit_message>
<xml_diff>
--- a/Benchmark-excel/benchmarkStatsV3.xlsx
+++ b/Benchmark-excel/benchmarkStatsV3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\p7\Benchmark-excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\p7\benchmark-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A77E4649-3932-48E3-9B70-1EEFA4C81CDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37478861-0AA0-4BE8-BB41-409404E90C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,6 @@
     <definedName name="Benchmarks.TicketedCodeRunnerBenchmark_report_1" localSheetId="5">samlet!$C$1:$D$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -2401,7 +2400,7 @@
           <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
-            <c:v>T=4,C=4</c:v>
+            <c:v>T=4, C=4</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -2617,7 +2616,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="da-DK"/>
-                  <a:t>Mean (ms</a:t>
+                  <a:t>Mean (ms)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -19807,8 +19806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" topLeftCell="E42" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="P50" sqref="P50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>